<commit_message>
excel sheet with advance formulas
</commit_message>
<xml_diff>
--- a/2_calculate_sales_using_advance_formula/advance_formula_sales_report.xlsx
+++ b/2_calculate_sales_using_advance_formula/advance_formula_sales_report.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd0102fde609f8b2/Documents/newfolder3/2_calculate_sales_using_advance_formula/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC10484C611C5F8C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51B5CEED-B45E-40EE-BD11-91A4B8B551DC}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC10484C611C5F8C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0EB11AC-5669-48D5-8FB1-3C7D333E7FF6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="advance_formula" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">advance_formula!$A$1:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -221,12 +224,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,6 +233,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,7 +529,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,10 +602,10 @@
       <c r="L3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="6"/>
+      <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -639,8 +642,8 @@
         <f>SUMIF(C2:C11,J4,D2:D11)</f>
         <v>43000</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -790,7 +793,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N15" s="12" t="s">
@@ -799,7 +802,7 @@
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F16" s="10"/>
+      <c r="F16" s="8"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
     </row>
@@ -807,37 +810,37 @@
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="6">
         <v>2</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="6">
         <v>3</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="6">
         <v>4</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="6">
         <v>5</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="6">
         <v>6</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="6">
         <v>7</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="6">
         <v>8</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="6">
         <v>9</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="6">
         <v>10</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="9" t="s">
         <v>0</v>
       </c>
       <c r="O17" s="5">
@@ -848,37 +851,37 @@
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="N18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="O18" s="5" t="str">
@@ -890,37 +893,37 @@
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="N19" s="9" t="s">
         <v>23</v>
       </c>
       <c r="O19" s="5" t="str">
@@ -932,37 +935,37 @@
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>15000</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="6">
         <v>18000</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <v>17500</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>13000</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="6">
         <v>23000</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="6">
         <v>25000</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="6">
         <v>20000</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="6">
         <v>18500</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="6">
         <v>14000</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="6">
         <v>8000</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="9" t="s">
         <v>3</v>
       </c>
       <c r="O20" s="5">
@@ -971,6 +974,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="N3:O4"/>
     <mergeCell ref="N15:O16"/>

</xml_diff>